<commit_message>
Add more scenarios Fix webdriver io check equas text function
</commit_message>
<xml_diff>
--- a/Testing notes/Testing strategy.xlsx
+++ b/Testing notes/Testing strategy.xlsx
@@ -9,8 +9,8 @@
   </bookViews>
   <sheets>
     <sheet name="Functional Test" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="Non Functional Testing" sheetId="2" state="visible" r:id="rId3"/>
-    <sheet name="tax relief calculation" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="tax relief calculation" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="Non Functional Testing" sheetId="3" state="visible" r:id="rId4"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="79">
   <si>
     <t xml:space="preserve">Remarks</t>
   </si>
@@ -200,7 +200,7 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">AC1: Able to retrieve a list that consists of </t>
+      <t xml:space="preserve">Able to retrieve a list that consists of </t>
     </r>
     <r>
       <rPr>
@@ -213,6 +213,12 @@
     </r>
   </si>
   <si>
+    <t xml:space="preserve">natid field must be masked from the 5th character onwards with dollar sign ‘$’</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Test calculation 1</t>
+  </si>
+  <si>
     <r>
       <rPr>
         <sz val="10"/>
@@ -220,32 +226,63 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">AC2: </t>
+      <t xml:space="preserve">Person 1 Expected: </t>
     </r>
     <r>
       <rPr>
         <sz val="10"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">1578
+Person 1 Actual: 1578.00
+Person 2 Expected: 2380
+Person 2 Actual: 2380.00</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Test calculation 2</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">natid field must be masked from the 5th character onwards with dollar sign ‘$’ </t>
+      <t xml:space="preserve">Expected</t>
     </r>
-  </si>
-  <si>
-    <t xml:space="preserve">AC3: The tax relief displayed must be correct based on the formula provided</t>
-  </si>
-  <si>
-    <t xml:space="preserve">AC4: Tax relief amount should be rounded to two decimal places by normal rounding rule</t>
-  </si>
-  <si>
-    <t xml:space="preserve">AC5: For tax relief amount more than 0.00 but less than 50.00, the final tax relief amount should be 50.00</t>
-  </si>
-  <si>
-    <t xml:space="preserve">AC5: For tax relief amount more than 50.00, the final tax amount should be the same amount</t>
-  </si>
-  <si>
-    <t xml:space="preserve">AC6: For tax relief amount more than 50.00 and before applying rounding comes with more than 2 decimal places, the value should be truncated at second decimal place and subject to normal rounding rule</t>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">: 928
+Actual: 927.62</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Test calculation 3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Expected: 50
+Actual: 50.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Test calculation 4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Expected: 601
+Actual: 601.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Test calculation 5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Expected: 3220
+Actual 3220.00</t>
   </si>
   <si>
     <t xml:space="preserve">Governor interface</t>
@@ -267,12 +304,6 @@
   </si>
   <si>
     <t xml:space="preserve">AC3: After clicking on the button, the page should redirect to a page with text that says “Cash dispensed”</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Verify average response time for endpoints</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Empty or invalid response should not throw error message that reveal the database schema</t>
   </si>
   <si>
     <t xml:space="preserve">Person</t>
@@ -297,7 +328,7 @@
 }</t>
   </si>
   <si>
-    <t xml:space="preserve">((4500-200)*0.367)+0 = 1578.10 -&gt; after rounding = 1578.00</t>
+    <t xml:space="preserve">((4500-200)*0.367)+0 = 1578.10 -&gt; after rounding = 1578</t>
   </si>
   <si>
     <t xml:space="preserve">Scenario 4.3 Person 2</t>
@@ -313,7 +344,77 @@
 }</t>
   </si>
   <si>
-    <t xml:space="preserve">((2400-50)*0.8)+500 = 2380.00</t>
+    <t xml:space="preserve">((2400-50)*0.8)+500 = 2380</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Scenario 4.4 Person 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{
+  "birthday": "26121945",
+  "gender": "F",
+  "name": "Mona Tan",
+  "natid": "S1673556F",
+  "salary": "1200.17",
+  "tax": "35"
+}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">((1200.17-35)*0.367)+500 = 927.61739 -&gt; 927.62 -&gt; 928</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Scenario 4.5 Person 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{
+  "birthday": "02041940",
+  "gender": "M",
+  "name": "Paul Koh",
+  "natid": "S5728351C",
+  "salary": "598.34",
+  "tax": "0"
+}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">((598.34-0)*0.05)+0) = 29.917 -&gt; 50</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Scenario 4.6 Person 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{
+  "birthday": "02041967",
+  "gender": "M",
+  "name": "Jason Chua",
+  "natid": "S3896611A",
+  "salary": "1938.55",
+  "tax": "300"
+}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">((1938.55-300)*0.367)+0) = 601.34785 -&gt; 601</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Scenario 4.7 Person 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{
+  "birthday": "01082000”,
+  "gender": "F",
+  "name": "Lisa Tan",
+  "natid": "S2091418A",
+  "salary": "4300.45",
+  "tax": "900"
+}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">((4300.45-900)*0.8)+500) = 3220.36 -&gt; 3220</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Verify average response time for endpoints</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Empty or invalid response should not throw error message that reveal the database schema</t>
   </si>
 </sst>
 </file>
@@ -456,7 +557,7 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>720</xdr:colOff>
+      <xdr:colOff>1080</xdr:colOff>
       <xdr:row>26</xdr:row>
       <xdr:rowOff>360</xdr:rowOff>
     </xdr:from>
@@ -464,7 +565,7 @@
       <xdr:col>5</xdr:col>
       <xdr:colOff>3095280</xdr:colOff>
       <xdr:row>26</xdr:row>
-      <xdr:rowOff>1875600</xdr:rowOff>
+      <xdr:rowOff>1875240</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -477,8 +578,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9322920" y="7023960"/>
-          <a:ext cx="3094560" cy="1875240"/>
+          <a:off x="9323280" y="7023960"/>
+          <a:ext cx="3094200" cy="1874880"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -500,8 +601,8 @@
   </sheetPr>
   <dimension ref="A1:F40"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C23" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D27" activeCellId="0" sqref="D27"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C29" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E39" activeCellId="0" sqref="E39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -611,7 +712,7 @@
       <c r="E7" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="F7" s="7" t="s">
+      <c r="F7" s="6" t="s">
         <v>15</v>
       </c>
     </row>
@@ -625,7 +726,7 @@
       <c r="E8" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="F8" s="7" t="s">
+      <c r="F8" s="6" t="s">
         <v>15</v>
       </c>
     </row>
@@ -639,7 +740,7 @@
       <c r="E9" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="F9" s="7" t="s">
+      <c r="F9" s="6" t="s">
         <v>15</v>
       </c>
     </row>
@@ -706,7 +807,7 @@
       <c r="E15" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="F15" s="7" t="s">
+      <c r="F15" s="6" t="s">
         <v>9</v>
       </c>
     </row>
@@ -720,7 +821,7 @@
       <c r="E16" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="F16" s="7" t="s">
+      <c r="F16" s="6" t="s">
         <v>9</v>
       </c>
     </row>
@@ -734,7 +835,7 @@
       <c r="E17" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="F17" s="7" t="s">
+      <c r="F17" s="6" t="s">
         <v>15</v>
       </c>
     </row>
@@ -784,7 +885,7 @@
       <c r="E22" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="F22" s="7" t="s">
+      <c r="F22" s="6" t="s">
         <v>32</v>
       </c>
     </row>
@@ -798,7 +899,7 @@
       <c r="E23" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="F23" s="7" t="s">
+      <c r="F23" s="6" t="s">
         <v>32</v>
       </c>
     </row>
@@ -849,11 +950,11 @@
       <c r="D29" s="3" t="n">
         <v>4.2</v>
       </c>
-      <c r="E29" s="1" t="s">
+      <c r="E29" s="4" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="30" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="2"/>
       <c r="B30" s="2"/>
       <c r="C30" s="5"/>
@@ -863,8 +964,11 @@
       <c r="E30" s="1" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F30" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="2"/>
       <c r="B31" s="2"/>
       <c r="C31" s="5"/>
@@ -872,10 +976,13 @@
         <v>4.4</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>42</v>
+      </c>
+      <c r="F31" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="2"/>
       <c r="B32" s="2"/>
       <c r="C32" s="5"/>
@@ -883,10 +990,13 @@
         <v>4.5</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>44</v>
+      </c>
+      <c r="F32" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="2"/>
       <c r="B33" s="2"/>
       <c r="C33" s="5"/>
@@ -894,7 +1004,10 @@
         <v>4.6</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>43</v>
+        <v>46</v>
+      </c>
+      <c r="F33" s="1" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -905,22 +1018,25 @@
         <v>4.7</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>44</v>
+        <v>48</v>
+      </c>
+      <c r="F34" s="1" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="57.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A37" s="2" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="B37" s="3" t="s">
         <v>2</v>
       </c>
       <c r="C37" s="3"/>
       <c r="D37" s="1" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="E37" s="4" t="s">
-        <v>47</v>
+        <v>52</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -933,7 +1049,7 @@
         <v>5.1</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -944,7 +1060,7 @@
         <v>5.2</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>49</v>
+        <v>54</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -955,7 +1071,7 @@
         <v>5.3</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>50</v>
+        <v>55</v>
       </c>
     </row>
   </sheetData>
@@ -985,10 +1101,117 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
+  <dimension ref="A1:C7"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A5" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="23.2"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="29.44"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="31.12"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="4" style="1" width="11.52"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="106.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="89.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="93.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="95.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>76</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
+      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1003,7 +1226,7 @@
         <v>1</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>51</v>
+        <v>77</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1011,7 +1234,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>52</v>
+        <v>78</v>
       </c>
     </row>
   </sheetData>
@@ -1023,67 +1246,4 @@
     <oddFooter>&amp;CPage &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:C3"/>
-  <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C4" activeCellId="0" sqref="C4"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="23.2"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="29.45"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="31.12"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="4" style="1" width="11.52"/>
-  </cols>
-  <sheetData>
-    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="106.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="89.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="B3" s="7" t="s">
-        <v>60</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>61</v>
-      </c>
-    </row>
-  </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
-  </headerFooter>
-</worksheet>
 </file>
</xml_diff>